<commit_message>
Added to ReadMe file, changed names of CSV, added to report
</commit_message>
<xml_diff>
--- a/Report_and_Presentation_Grading_Rubric_Checklist.xlsx
+++ b/Report_and_Presentation_Grading_Rubric_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/tpk5401_psu_edu/Documents/Courses/AERSP_424/Spring 2024/Project/For Students Reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="428" documentId="8_{2E687571-912A-48DF-A2AF-07FCC8CEC5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4ED0C7-209E-4612-9A8E-310948C6D00A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B846CFE9-7A0C-49B5-B471-509DD4A46920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-27345" yWindow="8205" windowWidth="25455" windowHeight="12765" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,7 +240,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -346,7 +346,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -499,21 +499,21 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,134 +527,171 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="D9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <f>SUM(B2:B13)</f>
         <v>15</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C3:C13)</f>
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small fixes to report and comments
</commit_message>
<xml_diff>
--- a/Report_and_Presentation_Grading_Rubric_Checklist.xlsx
+++ b/Report_and_Presentation_Grading_Rubric_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjgly\Downloads\Spring 2024\AERSP 424\Final Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B846CFE9-7A0C-49B5-B471-509DD4A46920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F29F1C-AF28-445F-BE0C-564BB4BDE427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27345" yWindow="8205" windowWidth="25455" windowHeight="12765" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,21 +499,21 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.52734375" customWidth="1"/>
+    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -541,7 +541,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -555,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -597,7 +597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -611,7 +611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -625,7 +625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -639,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -653,7 +653,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -667,7 +667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>

</xml_diff>